<commit_message>
udp, demo server ,fix
</commit_message>
<xml_diff>
--- a/cfgdata/struct/object.xlsx
+++ b/cfgdata/struct/object.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20265" windowHeight="9135"/>
+    <workbookView windowWidth="24180" windowHeight="10755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestObject" sheetId="1" r:id="rId1"/>
+    <sheet name="Player" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +65,54 @@
     <t>Increment</t>
   </si>
   <si>
+    <t>属性名</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>bool,int8,int16,
+int32,int64,uint8,
+uint16,uint32,uint64,
+string,float,double</t>
+  </si>
+  <si>
+    <t>默认值</t>
+  </si>
+  <si>
+    <t>改变通知自己</t>
+  </si>
+  <si>
+    <t>改变通知别人</t>
+  </si>
+  <si>
+    <t>改变通知事件</t>
+  </si>
+  <si>
+    <t>是否存数据库</t>
+  </si>
+  <si>
+    <t>是否主键</t>
+  </si>
+  <si>
+    <t>int
+bigint
+varchar
+timestamp</t>
+  </si>
+  <si>
+    <t>长度</t>
+  </si>
+  <si>
+    <t>数据库默认值</t>
+  </si>
+  <si>
+    <t>是否索引</t>
+  </si>
+  <si>
+    <t>是否自增</t>
+  </si>
+  <si>
     <t>pro1</t>
   </si>
   <si>
@@ -77,6 +126,36 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>等级</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>glod</t>
   </si>
 </sst>
 </file>
@@ -84,12 +163,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,22 +178,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.25"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -126,98 +236,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,14 +273,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -249,13 +314,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,7 +336,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.25"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +408,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,103 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,65 +528,41 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,16 +582,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,46 +605,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,6 +634,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -569,10 +662,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -581,147 +674,159 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,97 +1179,132 @@
   <sheetPr/>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="10.125" customWidth="1"/>
-    <col min="9" max="9" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="13.875" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
     <col min="11" max="11" width="10.375" customWidth="1"/>
     <col min="12" max="12" width="10.875" customWidth="1"/>
+    <col min="13" max="13" width="15.25" customWidth="1"/>
     <col min="14" max="14" width="10.625" customWidth="1"/>
     <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="33" customHeight="1" spans="1:16">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="3"/>
+    <row r="2" ht="60" customHeight="1" spans="1:16">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3"/>
+        <v>31</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -1180,10 +1320,10 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1204,18 +1344,295 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="7:7">
-      <c r="G9" s="2"/>
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <cols>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="6" max="6" width="11.25" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="19.75" customWidth="1"/>
+    <col min="10" max="10" width="9.75" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" ht="53" customHeight="1" spans="1:16">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:16">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>